<commit_message>
jdre-28/05/15-Se actualizo el documento BITACORA.xlsx con las actividades realizadas
</commit_message>
<xml_diff>
--- a/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/CUAT_2_MAY_AGO/PARCIAL_1/BITACORA.xlsx
+++ b/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/CUAT_2_MAY_AGO/PARCIAL_1/BITACORA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19440" windowHeight="8340"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19440" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>UNIVERSIDAD TECNOLÓGICA DEL  CENTRO DE VERACRUZ
 TECNOLOGÍAS DE LA INFORMACIÓN Y COMUNICACIÓN
@@ -192,6 +192,24 @@
   </si>
   <si>
     <t>Desarrollo de aplicaciones WEB</t>
+  </si>
+  <si>
+    <t>Reunion de equipo para opinar sobre el nombre de la compañía, inicio de desarrollo del sitio web empresarial</t>
+  </si>
+  <si>
+    <t>Se decidio que el nombre de la compañía sera DevUniverse y se continuara con el desarrollo del sitio web empresarial</t>
+  </si>
+  <si>
+    <t>Sitio WEB fase uno y bitacora</t>
+  </si>
+  <si>
+    <t>Finalizacion de la primera etapa del sitio WEB empresarial</t>
+  </si>
+  <si>
+    <t>Sitio WEB empresarial DevUniverse en espera de ser evaluado por el profesor lider Alejandro Lara San Juan</t>
+  </si>
+  <si>
+    <t>Sitio WEB empresarial</t>
   </si>
 </sst>
 </file>
@@ -199,7 +217,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="32" x14ac:knownFonts="1">
     <font>
@@ -821,7 +839,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="30" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -830,6 +848,33 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -848,27 +893,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -876,12 +900,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="30" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1304,7 +1322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1334,46 +1352,46 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="29"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="38"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="29"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="38"/>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="29"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="38"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1396,13 +1414,13 @@
       <c r="C6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
@@ -1414,13 +1432,13 @@
       <c r="C7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -1432,13 +1450,13 @@
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -1450,13 +1468,13 @@
       <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
@@ -1468,13 +1486,13 @@
       <c r="C10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="31">
         <v>1</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
@@ -1486,13 +1504,13 @@
       <c r="C11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
@@ -1518,11 +1536,11 @@
       <c r="C13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
@@ -1534,13 +1552,13 @@
       <c r="C14" s="17">
         <v>1</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
@@ -1552,13 +1570,13 @@
       <c r="C15" s="17">
         <v>2</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
@@ -1570,13 +1588,13 @@
       <c r="C16" s="17">
         <v>3</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
@@ -1588,13 +1606,13 @@
       <c r="C17" s="17">
         <v>4</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
@@ -1606,11 +1624,11 @@
       <c r="C18" s="17">
         <v>5</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
@@ -1622,11 +1640,11 @@
       <c r="C19" s="17">
         <v>6</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
@@ -1648,6 +1666,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:K4"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="D9:H9"/>
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:H17"/>
     <mergeCell ref="D18:H18"/>
@@ -1657,11 +1680,6 @@
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="D14:H14"/>
     <mergeCell ref="D15:H15"/>
-    <mergeCell ref="B2:K4"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="D9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1672,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1717,42 +1735,42 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="44"/>
       <c r="J3" s="13"/>
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
       <c r="J4" s="13"/>
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="42"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
       <c r="J5" s="13"/>
       <c r="K5" s="6"/>
     </row>
@@ -1831,7 +1849,7 @@
       <c r="G9" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="28" t="s">
         <v>45</v>
       </c>
       <c r="I9" s="21"/>
@@ -1858,7 +1876,7 @@
       <c r="G10" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="44" t="s">
+      <c r="H10" s="28" t="s">
         <v>49</v>
       </c>
       <c r="I10" s="21"/>
@@ -1885,7 +1903,7 @@
       <c r="G11" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="44" t="s">
+      <c r="H11" s="28" t="s">
         <v>49</v>
       </c>
       <c r="I11" s="21"/>
@@ -1894,26 +1912,54 @@
     </row>
     <row r="12" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="B12" s="22">
+        <v>4</v>
+      </c>
+      <c r="C12" s="24">
+        <v>42149</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="I12" s="21"/>
       <c r="J12" s="2"/>
       <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
+      <c r="B13" s="22">
+        <v>4</v>
+      </c>
+      <c r="C13" s="24">
+        <v>42152</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="I13" s="21"/>
       <c r="J13" s="2"/>
       <c r="K13" s="11"/>
@@ -1973,7 +2019,7 @@
     <row r="18" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="22"/>
-      <c r="C18" s="43"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="19"/>
       <c r="E18" s="22"/>
       <c r="F18" s="25"/>

</xml_diff>